<commit_message>
Removed the note about real cryptocurrency funds for the demo terminal
</commit_message>
<xml_diff>
--- a/ExchangeCalculation.xlsx
+++ b/ExchangeCalculation.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ExchangeBroker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\exchange-broker\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEC9286-9919-432F-B905-93DC3EC37B65}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>GRFT rate:</t>
   </si>
@@ -45,9 +46,6 @@
   </si>
   <si>
     <t>fee</t>
-  </si>
-  <si>
-    <t>rfee</t>
   </si>
   <si>
     <t>SellFiatAmount (USD)</t>
@@ -65,12 +63,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
-    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.0000000000"/>
-    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00000"/>
-    <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00000000"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00000"/>
+    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -184,13 +182,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -211,7 +209,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -220,10 +218,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -505,31 +503,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" style="7" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" style="7" customWidth="1"/>
     <col min="16" max="16" width="15" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -543,44 +541,41 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="7">
         <v>6500</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="8">
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="8">
         <v>10</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K4" s="8">
         <v>1.5499999999999999E-3</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O4" s="8">
         <v>1111.1111111111099</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="9"/>
       <c r="F5" s="1"/>
@@ -590,7 +585,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -648,7 +643,7 @@
         <v>10.075566750629712</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -706,7 +701,7 @@
         <v>10.075566750629712</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -764,7 +759,7 @@
         <v>7.556675062972272E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>

</xml_diff>